<commit_message>
Second Commit with report change
</commit_message>
<xml_diff>
--- a/BasicFrameWork/DataFolder/TestingData.xlsx
+++ b/BasicFrameWork/DataFolder/TestingData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304965\IdeaProjects\SeleniumTesting\DataFolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\303785\git\BasicTestFrameWork\BasicFrameWork\DataFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF5A665-D0DA-451F-AC9E-9357287FDC2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="1650" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="4550" yWindow="1650" windowWidth="15380" windowHeight="7880" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -127,17 +128,19 @@
     <t>Mahindra</t>
   </si>
   <si>
-    <t>MotorVehicles</t>
-  </si>
-  <si>
-    <t>Eg</t>
+    <t>Aks</t>
+  </si>
+  <si>
+    <t>TATA</t>
+  </si>
+  <si>
+    <t>Canara Bank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -463,23 +466,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="99" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="100" max="999" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="1000" max="9999" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="10000" max="16384" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="9" width="11" customWidth="1" collapsed="1"/>
+    <col min="10" max="99" width="12" customWidth="1" collapsed="1"/>
+    <col min="100" max="999" width="13" customWidth="1" collapsed="1"/>
+    <col min="1000" max="9999" width="14" customWidth="1" collapsed="1"/>
+    <col min="10000" max="16384" width="15" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -507,7 +510,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -515,7 +518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -523,7 +526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -537,7 +540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -551,7 +554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -572,14 +575,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,16 +602,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -628,14 +631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -655,14 +658,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -682,14 +685,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -717,7 +720,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -731,7 +734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -745,7 +748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -765,16 +768,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -782,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -790,7 +793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>33</v>
       </c>
@@ -798,7 +801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>10</v>
       </c>
@@ -812,22 +815,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -841,9 +844,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -855,7 +858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -869,15 +872,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -895,22 +898,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -924,7 +927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -938,7 +941,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -952,7 +955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -960,7 +963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>

</xml_diff>